<commit_message>
Se corrigieron algunos porcentajes
</commit_message>
<xml_diff>
--- a/documentacion/Documentos del Proyecto/RPT1 Reporte Evaluacion Estandar Codificacion.xlsx
+++ b/documentacion/Documentos del Proyecto/RPT1 Reporte Evaluacion Estandar Codificacion.xlsx
@@ -409,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M86" authorId="0">
+    <comment ref="M88" authorId="0">
       <text>
         <r>
           <rPr>
@@ -423,7 +423,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M89" authorId="0">
+    <comment ref="M92" authorId="0">
       <text>
         <r>
           <rPr>
@@ -437,7 +437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M92" authorId="0">
+    <comment ref="M96" authorId="0">
       <text>
         <r>
           <rPr>
@@ -465,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M95" authorId="0">
+    <comment ref="M100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -489,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M98" authorId="0">
+    <comment ref="M104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -518,7 +518,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
   <si>
     <t>Translation</t>
   </si>
@@ -874,9 +874,6 @@
     <t>Sentencias 'throw' redundantes</t>
   </si>
   <si>
-    <t>Clases que no se diseñaron bien como para ser extendidas</t>
-  </si>
-  <si>
     <t>Atrib. non-final y non-static que no se defin como 'private'</t>
   </si>
   <si>
@@ -905,13 +902,28 @@
   </si>
   <si>
     <t>A partir del estándar "Code Conventions for the Java Programming Language", se ha analizado cada aspecto definido por la Convención, sobre los cuatro proyectos pertenecientes a la aplicación, es decir sobre las 16060 líneas de código y se obtuvieron los siguientes resultados:</t>
+  </si>
+  <si>
+    <t>Total de 'switch' en el sistema</t>
+  </si>
+  <si>
+    <t>Total de 'throw' en el sistema</t>
+  </si>
+  <si>
+    <t>Métodos que no se diseñaron bien como para ser extendidos</t>
+  </si>
+  <si>
+    <t>Cantidad de métodos</t>
+  </si>
+  <si>
+    <t>Cantidad de atributos no estáticos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -965,6 +977,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1204,7 +1223,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1249,8 +1268,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1267,6 +1284,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -9367,10 +9390,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N99"/>
+  <dimension ref="A1:N118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView tabSelected="1" topLeftCell="F73" workbookViewId="0">
+      <selection activeCell="M98" sqref="M98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9386,38 +9409,38 @@
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" customWidth="1"/>
     <col min="11" max="11" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="63.5703125" customWidth="1"/>
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="M1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="M2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="M5" s="32" t="s">
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="M5" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="32"/>
+      <c r="N5" s="30"/>
     </row>
     <row r="6" spans="1:14" ht="16.5" customHeight="1"/>
     <row r="7" spans="1:14">
@@ -9438,10 +9461,10 @@
       <c r="K7" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="M7" s="30" t="s">
+      <c r="M7" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="N7" s="30">
+      <c r="N7" s="28">
         <f>K8+K10+K15+K17+K18+K11+K16</f>
         <v>2734</v>
       </c>
@@ -9467,10 +9490,10 @@
         <f>C8+E8+G8+I8</f>
         <v>28</v>
       </c>
-      <c r="M8" s="30" t="s">
+      <c r="M8" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="N8" s="30">
+      <c r="N8" s="28">
         <f>K34</f>
         <v>2045</v>
       </c>
@@ -9495,10 +9518,10 @@
         <f>C9+E9+G9+I9</f>
         <v>16060</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="44">
         <f>N8/N7</f>
         <v>0.74798829553767376</v>
       </c>
@@ -9544,10 +9567,10 @@
         <f t="shared" ref="K11:K19" si="0">C11+E11+G11+I11</f>
         <v>569</v>
       </c>
-      <c r="M11" s="30" t="s">
+      <c r="M11" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="N11" s="30">
+      <c r="N11" s="28">
         <f>K12</f>
         <v>39</v>
       </c>
@@ -9572,10 +9595,10 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="N12" s="30">
+      <c r="N12" s="28">
         <f>K28</f>
         <v>36</v>
       </c>
@@ -9600,10 +9623,10 @@
         <f t="shared" si="0"/>
         <v>8058</v>
       </c>
-      <c r="M13" s="30" t="s">
+      <c r="M13" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N13" s="31">
+      <c r="N13" s="44">
         <f>N12/N11</f>
         <v>0.92307692307692313</v>
       </c>
@@ -9649,10 +9672,10 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="M15" s="30" t="s">
+      <c r="M15" s="28" t="s">
         <v>86</v>
       </c>
-      <c r="N15" s="30">
+      <c r="N15" s="28">
         <f>K16+K11</f>
         <v>743</v>
       </c>
@@ -9677,10 +9700,10 @@
         <f t="shared" si="0"/>
         <v>174</v>
       </c>
-      <c r="M16" s="30" t="s">
+      <c r="M16" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="N16" s="30">
+      <c r="N16" s="28">
         <f>K36</f>
         <v>707</v>
       </c>
@@ -9705,10 +9728,10 @@
         <f>C17+E17+G17+I17</f>
         <v>1701</v>
       </c>
-      <c r="M17" s="30" t="s">
+      <c r="M17" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N17" s="31">
+      <c r="N17" s="44">
         <f>N16/N15</f>
         <v>0.95154777927321665</v>
       </c>
@@ -9754,58 +9777,58 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="M19" s="30" t="s">
+      <c r="M19" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="N19" s="30">
+      <c r="N19" s="28">
         <f>K18+K10</f>
         <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:14">
-      <c r="M20" s="30" t="s">
+      <c r="M20" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="N20" s="30">
+      <c r="N20" s="28">
         <f>K35</f>
         <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:14">
-      <c r="M21" s="30" t="s">
+      <c r="M21" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N21" s="31">
+      <c r="N21" s="44">
         <f>N20/N19</f>
         <v>0.64736842105263159</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="M23" s="30" t="s">
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="37"/>
+      <c r="K23" s="37"/>
+      <c r="M23" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="N23" s="30">
+      <c r="N23" s="28">
         <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" thickBot="1">
-      <c r="M24" s="30" t="s">
+      <c r="M24" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="N24" s="30">
+      <c r="N24" s="28">
         <f>K37</f>
         <v>64</v>
       </c>
@@ -9813,7 +9836,7 @@
     <row r="25" spans="1:14">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="38" t="s">
         <v>57</v>
       </c>
       <c r="E25" s="21" t="s">
@@ -9828,16 +9851,16 @@
       <c r="K25" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="M25" s="30" t="s">
+      <c r="M25" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N25" s="31">
+      <c r="N25" s="29">
         <f>N24/N23</f>
         <v>0.26229508196721313</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="15.75" thickBot="1">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="39" t="s">
         <v>79</v>
       </c>
       <c r="B26" s="11"/>
@@ -9873,10 +9896,10 @@
         <v>80</v>
       </c>
       <c r="K27" s="3"/>
-      <c r="M27" s="30" t="s">
+      <c r="M27" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="N27" s="30">
+      <c r="N27" s="28">
         <f>K9</f>
         <v>16060</v>
       </c>
@@ -9902,10 +9925,10 @@
         <f t="shared" ref="K28:K59" si="1">C28+E28+G28+I28</f>
         <v>36</v>
       </c>
-      <c r="M28" s="30" t="s">
+      <c r="M28" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="N28" s="30">
+      <c r="N28" s="28">
         <f>K33</f>
         <v>1381</v>
       </c>
@@ -9931,10 +9954,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M29" s="30" t="s">
+      <c r="M29" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N29" s="31">
+      <c r="N29" s="29">
         <f>N28/N27</f>
         <v>8.5990037359900379E-2</v>
       </c>
@@ -9982,10 +10005,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M31" s="30" t="s">
+      <c r="M31" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="N31" s="30">
+      <c r="N31" s="28">
         <f>K11</f>
         <v>569</v>
       </c>
@@ -10011,10 +10034,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M32" s="30" t="s">
+      <c r="M32" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="N32" s="30">
+      <c r="N32" s="28">
         <f>K41</f>
         <v>17</v>
       </c>
@@ -10040,10 +10063,10 @@
         <f t="shared" si="1"/>
         <v>1381</v>
       </c>
-      <c r="M33" s="30" t="s">
+      <c r="M33" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N33" s="31">
+      <c r="N33" s="29">
         <f>N32/N31</f>
         <v>2.9876977152899824E-2</v>
       </c>
@@ -10091,10 +10114,10 @@
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="M35" s="30" t="s">
+      <c r="M35" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="N35" s="30">
+      <c r="N35" s="28">
         <f>K17+K8</f>
         <v>1729</v>
       </c>
@@ -10120,10 +10143,10 @@
         <f t="shared" si="1"/>
         <v>707</v>
       </c>
-      <c r="M36" s="30" t="s">
+      <c r="M36" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="N36" s="30">
+      <c r="N36" s="28">
         <f>K42</f>
         <v>7</v>
       </c>
@@ -10149,10 +10172,10 @@
         <f t="shared" si="1"/>
         <v>64</v>
       </c>
-      <c r="M37" s="30" t="s">
+      <c r="M37" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N37" s="31">
+      <c r="N37" s="29">
         <f>N36/N35</f>
         <v>4.048582995951417E-3</v>
       </c>
@@ -10200,10 +10223,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M39" s="30" t="s">
+      <c r="M39" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="N39" s="30">
+      <c r="N39" s="28">
         <f>K8</f>
         <v>28</v>
       </c>
@@ -10229,10 +10252,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M40" s="30" t="s">
+      <c r="M40" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="N40" s="30">
+      <c r="N40" s="28">
         <f>K45</f>
         <v>2</v>
       </c>
@@ -10258,10 +10281,10 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="M41" s="30" t="s">
+      <c r="M41" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N41" s="31">
+      <c r="N41" s="29">
         <f>N40/N39</f>
         <v>7.1428571428571425E-2</v>
       </c>
@@ -10309,10 +10332,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M43" s="30" t="s">
+      <c r="M43" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="N43" s="30">
+      <c r="N43" s="28">
         <v>1655</v>
       </c>
     </row>
@@ -10337,10 +10360,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="M44" s="30" t="s">
+      <c r="M44" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="N44" s="30">
+      <c r="N44" s="28">
         <f>K47</f>
         <v>24</v>
       </c>
@@ -10366,10 +10389,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M45" s="30" t="s">
+      <c r="M45" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N45" s="31">
+      <c r="N45" s="29">
         <f>N44/N43</f>
         <v>1.4501510574018127E-2</v>
       </c>
@@ -10417,10 +10440,10 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="M47" s="30" t="s">
+      <c r="M47" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="N47" s="30">
+      <c r="N47" s="28">
         <f>N43</f>
         <v>1655</v>
       </c>
@@ -10446,10 +10469,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M48" s="30" t="s">
+      <c r="M48" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="N48" s="30">
+      <c r="N48" s="28">
         <f>K50</f>
         <v>3</v>
       </c>
@@ -10475,10 +10498,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M49" s="30" t="s">
+      <c r="M49" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N49" s="31">
+      <c r="N49" s="29">
         <f>N48/N47</f>
         <v>1.8126888217522659E-3</v>
       </c>
@@ -10526,10 +10549,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M51" s="30" t="s">
+      <c r="M51" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="N51" s="30">
+      <c r="N51" s="28">
         <f>N35</f>
         <v>1729</v>
       </c>
@@ -10555,10 +10578,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M52" s="30" t="s">
+      <c r="M52" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="N52" s="30">
+      <c r="N52" s="28">
         <f>K53</f>
         <v>2</v>
       </c>
@@ -10584,10 +10607,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M53" s="30" t="s">
+      <c r="M53" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N53" s="31">
+      <c r="N53" s="29">
         <f>N52/N51</f>
         <v>1.1567379988432619E-3</v>
       </c>
@@ -10635,10 +10658,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M55" s="30" t="s">
+      <c r="M55" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="N55" s="30">
+      <c r="N55" s="28">
         <f>K13</f>
         <v>8058</v>
       </c>
@@ -10664,10 +10687,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M56" s="30" t="s">
+      <c r="M56" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="N56" s="30">
+      <c r="N56" s="28">
         <f>K61</f>
         <v>423</v>
       </c>
@@ -10693,10 +10716,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="M57" s="30" t="s">
+      <c r="M57" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N57" s="31">
+      <c r="N57" s="29">
         <f>N56/N55</f>
         <v>5.2494415487714073E-2</v>
       </c>
@@ -10744,10 +10767,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M59" s="30" t="s">
+      <c r="M59" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="N59" s="30">
+      <c r="N59" s="28">
         <f>K13</f>
         <v>8058</v>
       </c>
@@ -10773,10 +10796,10 @@
         <f t="shared" ref="K60:K90" si="2">C60+E60+G60+I60</f>
         <v>0</v>
       </c>
-      <c r="M60" s="30" t="s">
+      <c r="M60" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="N60" s="30">
+      <c r="N60" s="28">
         <f>K62</f>
         <v>738</v>
       </c>
@@ -10802,10 +10825,10 @@
         <f t="shared" si="2"/>
         <v>423</v>
       </c>
-      <c r="M61" s="30" t="s">
+      <c r="M61" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N61" s="31">
+      <c r="N61" s="29">
         <f>N60/N59</f>
         <v>9.1586001489203275E-2</v>
       </c>
@@ -10853,10 +10876,10 @@
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="M63" s="30" t="s">
+      <c r="M63" s="28" t="s">
         <v>87</v>
       </c>
-      <c r="N63" s="30">
+      <c r="N63" s="28">
         <f>N7</f>
         <v>2734</v>
       </c>
@@ -10882,10 +10905,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M64" s="30" t="s">
+      <c r="M64" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="N64" s="30">
+      <c r="N64" s="28">
         <f>K63</f>
         <v>6</v>
       </c>
@@ -10911,10 +10934,10 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M65" s="30" t="s">
+      <c r="M65" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="N65" s="31">
+      <c r="N65" s="29">
         <f>N64/N63</f>
         <v>2.1945866861741038E-3</v>
       </c>
@@ -11459,8 +11482,8 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M85" s="22"/>
-      <c r="N85" s="17"/>
+      <c r="M85" s="40"/>
+      <c r="N85" s="41"/>
     </row>
     <row r="86" spans="1:14">
       <c r="A86" s="19" t="s">
@@ -11483,13 +11506,6 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="M86" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="N86" s="26">
-        <f>K78</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="87" spans="1:14">
       <c r="A87" s="5" t="s">
@@ -11512,12 +11528,11 @@
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="M87" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="N87" s="27">
-        <f>N86/$K$13</f>
-        <v>4.9640109208240262E-4</v>
+      <c r="M87" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="N87" s="42">
+        <v>4</v>
       </c>
     </row>
     <row r="88" spans="1:14">
@@ -11541,8 +11556,13 @@
         <f t="shared" si="2"/>
         <v>1197</v>
       </c>
-      <c r="M88" s="22"/>
-      <c r="N88" s="17"/>
+      <c r="M88" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="N88" s="42">
+        <f>K78</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="89" spans="1:14">
       <c r="A89" s="5" t="s">
@@ -11565,12 +11585,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M89" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="N89" s="26">
-        <f>K79</f>
-        <v>8</v>
+      <c r="M89" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="N89" s="45">
+        <f>N88/N87</f>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:14">
@@ -11594,99 +11614,159 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M90" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="N90" s="27">
-        <f>N89/$K$13</f>
-        <v>9.9280218416480524E-4</v>
-      </c>
+      <c r="M90" s="8"/>
+      <c r="N90" s="8"/>
     </row>
     <row r="91" spans="1:14">
-      <c r="M91" s="22"/>
-      <c r="N91" s="17"/>
+      <c r="M91" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="N91" s="42">
+        <v>69</v>
+      </c>
     </row>
     <row r="92" spans="1:14">
-      <c r="A92" s="34" t="s">
-        <v>121</v>
-      </c>
-      <c r="B92" s="33"/>
-      <c r="C92" s="33"/>
-      <c r="M92" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="N92" s="26">
+      <c r="A92" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="B92" s="31"/>
+      <c r="C92" s="31"/>
+      <c r="M92" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="N92" s="42">
+        <f>K79</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14">
+      <c r="M93" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="N93" s="43">
+        <f>N92/N91</f>
+        <v>0.11594202898550725</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14">
+      <c r="M94" s="8"/>
+      <c r="N94" s="8"/>
+    </row>
+    <row r="95" spans="1:14" ht="15.75">
+      <c r="A95" s="35" t="s">
+        <v>123</v>
+      </c>
+      <c r="M95" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="N95" s="42">
+        <f>N35</f>
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="96" spans="1:14">
+      <c r="A96" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="M96" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="N96" s="42">
         <f>K82</f>
         <v>1539</v>
       </c>
     </row>
-    <row r="93" spans="1:14">
-      <c r="M93" s="25" t="s">
+    <row r="97" spans="1:14">
+      <c r="A97" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="M97" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="N93" s="27">
-        <f>N92/$K$13</f>
-        <v>0.1909903201787044</v>
+      <c r="N97" s="45">
+        <f>N96/N95</f>
+        <v>0.89010989010989006</v>
       </c>
     </row>
-    <row r="94" spans="1:14">
-      <c r="M94" s="22"/>
-      <c r="N94" s="17"/>
+    <row r="98" spans="1:14">
+      <c r="A98" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="M98" s="8"/>
+      <c r="N98" s="8"/>
     </row>
-    <row r="95" spans="1:14" ht="15.75">
-      <c r="A95" s="37" t="s">
+    <row r="99" spans="1:14">
+      <c r="A99" s="34" t="s">
         <v>124</v>
       </c>
-      <c r="M95" s="25" t="s">
-        <v>119</v>
-      </c>
-      <c r="N95" s="26">
+      <c r="M99" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="N99" s="42">
+        <f>K11</f>
+        <v>569</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
+      <c r="M100" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="N100" s="42">
         <f>K86</f>
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:14">
-      <c r="A96" s="35" t="s">
-        <v>126</v>
-      </c>
-      <c r="M96" s="25" t="s">
+    <row r="101" spans="1:14">
+      <c r="M101" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="N96" s="27">
-        <f>N95/$K$13</f>
-        <v>1.9856043683296105E-3</v>
+      <c r="N101" s="43">
+        <f>N100/N99</f>
+        <v>2.8119507908611598E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:14">
-      <c r="A97" s="35" t="s">
-        <v>122</v>
-      </c>
-      <c r="M97" s="22"/>
-      <c r="N97" s="17"/>
+    <row r="103" spans="1:14">
+      <c r="M103" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="N103" s="42">
+        <f>N35</f>
+        <v>1729</v>
+      </c>
     </row>
-    <row r="98" spans="1:14">
-      <c r="A98" s="35" t="s">
-        <v>123</v>
-      </c>
-      <c r="M98" s="25" t="s">
-        <v>120</v>
-      </c>
-      <c r="N98" s="26">
+    <row r="104" spans="1:14">
+      <c r="M104" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="N104" s="42">
         <f>K88</f>
         <v>1197</v>
       </c>
     </row>
-    <row r="99" spans="1:14">
-      <c r="A99" s="36" t="s">
-        <v>125</v>
-      </c>
-      <c r="M99" s="28" t="s">
+    <row r="105" spans="1:14">
+      <c r="M105" s="42" t="s">
         <v>81</v>
       </c>
-      <c r="N99" s="29">
-        <f>N98/$K$13</f>
+      <c r="N105" s="43">
+        <f>N104/$K$13</f>
         <v>0.14854802680565898</v>
       </c>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="M109" s="8"/>
+      <c r="N109" s="8"/>
+    </row>
+    <row r="113" spans="13:14">
+      <c r="M113" s="8"/>
+      <c r="N113" s="8"/>
+    </row>
+    <row r="114" spans="13:14">
+      <c r="M114" s="8"/>
+      <c r="N114" s="8"/>
+    </row>
+    <row r="118" spans="13:14">
+      <c r="M118" s="8"/>
+      <c r="N118" s="8"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Formato y redaccion de conclusion
</commit_message>
<xml_diff>
--- a/documentacion/Documentos del Proyecto/RPT1 Reporte Evaluacion Estandar Codificacion.xlsx
+++ b/documentacion/Documentos del Proyecto/RPT1 Reporte Evaluacion Estandar Codificacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11535" windowHeight="5580" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="11535" windowHeight="5580"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="2" r:id="rId1"/>
@@ -16,6 +16,494 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>La Poderoza</author>
+  </authors>
+  <commentList>
+    <comment ref="A14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>JavadocMethod</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D14" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>WhitespaceAfter</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>JavadocPackage</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D18" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ModifierOrder</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>JavadocVariable</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D22" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>EmptyBlock</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>NeedBraces:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Ejemplo 'if' construct must use '{}'s.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>JavadocType</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RightCurly</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La búsqueda se hizo con el Eclipse y la siguiente clave:
+/\*\* . Resultado 244 ocurrencias.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>JavadocStyle</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D31" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AvoidInlineConditionals</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RegexpSingleline</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>EmptyStatement</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MagicNumber</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MemberName:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Aplica a atributos "non-static". Debe respetar el patrón '^[a-z][a-zA-Z0-9]*$'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MethodName:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Debe respetar el patrón '^[a-z][a-zA-Z0-9]*$'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D42" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>MissingSwitchDefault</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>StaticVariableName:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Aplica a atributos "static, non-final". Debe respetar el patrón '^[a-z][a-zA-Z0-9]*$'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D46" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>RedundantThrows</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>La búsqueda se hizo con el Eclipse y la siguiente clave:
+'import ' (sin comillas). Resultado 1655 ocurrencias.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AvoidStarImport</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D50" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DesignForExtension:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+La regla exacta dice que los métodos non-private y non-static que pueden ser subclaseados deben ser, o bien
+- abstract, o bien
+- final, o bien
+- tener una implementación vacía.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>UnusedImports</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D54" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>VisibilityModifier:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Only static final members may be public; other class members must be private.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>ParameterNumber</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D58" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>FinalParameters:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Changing the value of parameters during the execution of the method's algorithm can be confusing and should be avoided.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A62" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>WhitespaceAfter</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>La Poderoza</author>
@@ -518,7 +1006,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="137">
   <si>
     <t>Translation</t>
   </si>
@@ -901,9 +1389,6 @@
     <t>Reporte de evaluación del estándar de codificación</t>
   </si>
   <si>
-    <t>A partir del estándar "Code Conventions for the Java Programming Language", se ha analizado cada aspecto definido por la Convención, sobre los cuatro proyectos pertenecientes a la aplicación, es decir sobre las 16060 líneas de código y se obtuvieron los siguientes resultados:</t>
-  </si>
-  <si>
     <t>Total de 'switch' en el sistema</t>
   </si>
   <si>
@@ -917,13 +1402,28 @@
   </si>
   <si>
     <t>Cantidad de atributos no estáticos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A partir del estándar "Code Conventions for the Java Programming Language", se ha analizado cada aspecto definido por la Convención, </t>
+  </si>
+  <si>
+    <t>sobre los cuatro proyectos pertenecientes a la aplicación, es decir sobre las 16060 líneas de código y se obtuvieron los siguientes resultados:</t>
+  </si>
+  <si>
+    <t>Sobre las reglas de la Convención que fueron relevadas, 6 superan el 65% de desvío. Mientras que en las 20 reglas restantes el porcentaje no supera el 26%.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Por lo que se concluye que, teniendo en cuenta que sobre  26 reglas relevadas, 20 no supera un desvío del %25 y teniendo en cuenta las métricas de conteo de </t>
+  </si>
+  <si>
+    <t>objetos utilizadas, el código cumple con la convención en un:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,6 +1484,19 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1223,7 +1736,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1290,6 +1803,11 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -9378,22 +9896,624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="48.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="31" customFormat="1" ht="18.75">
+      <c r="A1" s="46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" s="48">
+        <f>20/26</f>
+        <v>0.76923076923076927</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="47"/>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="28">
+        <v>2734</v>
+      </c>
+      <c r="D13" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="E13" s="28">
+        <v>8058</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="28">
+        <v>2045</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E14" s="28">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="44">
+        <v>0.74798829553767376</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="29">
+        <v>9.1586001489203275E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="28">
+        <v>39</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="E17" s="28">
+        <v>2734</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="28">
+        <v>36</v>
+      </c>
+      <c r="D18" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E18" s="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="44">
+        <v>0.92307692307692313</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="29">
+        <v>2.1945866861741038E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="B21" s="28">
+        <v>743</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="24">
+        <v>8058</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="28">
+        <v>707</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="E22" s="26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="44">
+        <v>0.95154777927321665</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="27">
+        <v>1.1169024571854058E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="D24" s="22"/>
+      <c r="E24" s="17"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="28" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="28">
+        <v>190</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="26">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="28">
+        <v>123</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E26" s="27">
+        <v>1.2410027302060065E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B27" s="44">
+        <v>0.64736842105263159</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="D28" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="26">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29" s="28">
+        <v>244</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E29" s="27">
+        <v>1.4023330851327873E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="28">
+        <v>64</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="17"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="29">
+        <v>0.26229508196721313</v>
+      </c>
+      <c r="D31" s="25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E31" s="26">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="D32" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="27">
+        <v>4.8399106478034248E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B33" s="28">
+        <v>16060</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="17"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="28">
+        <v>1381</v>
+      </c>
+      <c r="D34" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="E34" s="26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="29">
+        <v>8.5990037359900379E-2</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E35" s="27">
+        <v>3.7230081906180194E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="D36" s="22"/>
+      <c r="E36" s="17"/>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="28">
+        <v>569</v>
+      </c>
+      <c r="D37" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="26">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="28">
+        <v>17</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" s="27">
+        <v>1.5388433854554479E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B39" s="29">
+        <v>2.9876977152899824E-2</v>
+      </c>
+      <c r="D39" s="40"/>
+      <c r="E39" s="41"/>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="28">
+        <v>1729</v>
+      </c>
+      <c r="D41" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="E41" s="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="28">
+        <v>7</v>
+      </c>
+      <c r="D42" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="29">
+        <v>4.048582995951417E-3</v>
+      </c>
+      <c r="D43" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E43" s="45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="D44" s="8"/>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="28">
+        <v>28</v>
+      </c>
+      <c r="D45" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="42">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="28">
+        <v>2</v>
+      </c>
+      <c r="D46" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B47" s="29">
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" s="43">
+        <v>0.11594202898550725</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B49" s="28">
+        <v>1655</v>
+      </c>
+      <c r="D49" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E49" s="42">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" s="28">
+        <v>24</v>
+      </c>
+      <c r="D50" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="E50" s="42">
+        <v>1539</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B51" s="29">
+        <v>1.4501510574018127E-2</v>
+      </c>
+      <c r="D51" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E51" s="45">
+        <v>0.89010989010989006</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="B53" s="28">
+        <v>1655</v>
+      </c>
+      <c r="D53" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="E53" s="42">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="28">
+        <v>3</v>
+      </c>
+      <c r="D54" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="42">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="29">
+        <v>1.8126888217522659E-3</v>
+      </c>
+      <c r="D55" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E55" s="43">
+        <v>2.8119507908611598E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" s="28">
+        <v>1729</v>
+      </c>
+      <c r="D57" s="42" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="42">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B58" s="28">
+        <v>2</v>
+      </c>
+      <c r="D58" s="42" t="s">
+        <v>119</v>
+      </c>
+      <c r="E58" s="42">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B59" s="29">
+        <v>1.1567379988432619E-3</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="E59" s="43">
+        <v>0.14854802680565898</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="B61" s="28">
+        <v>8058</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B62" s="28">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="29">
+        <v>5.2494415487714073E-2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N118"/>
+  <dimension ref="A5:N118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F73" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9413,16 +10533,6 @@
     <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="M1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="M2" t="s">
-        <v>127</v>
-      </c>
-    </row>
     <row r="5" spans="1:14" ht="15.75">
       <c r="A5" s="36" t="s">
         <v>63</v>
@@ -11529,7 +12639,7 @@
         <v>2</v>
       </c>
       <c r="M87" s="42" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N87" s="42">
         <v>4</v>
@@ -11619,7 +12729,7 @@
     </row>
     <row r="91" spans="1:14">
       <c r="M91" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N91" s="42">
         <v>69</v>
@@ -11657,7 +12767,7 @@
         <v>123</v>
       </c>
       <c r="M95" s="42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N95" s="42">
         <f>N35</f>
@@ -11669,7 +12779,7 @@
         <v>125</v>
       </c>
       <c r="M96" s="42" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N96" s="42">
         <f>K82</f>
@@ -11700,7 +12810,7 @@
         <v>124</v>
       </c>
       <c r="M99" s="42" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N99" s="42">
         <f>K11</f>
@@ -11727,7 +12837,7 @@
     </row>
     <row r="103" spans="1:14">
       <c r="M103" s="42" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N103" s="42">
         <f>N35</f>

</xml_diff>